<commit_message>
added all necesary tests
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fa8db44bbb22994a/Escritorio/Cosas/Cosas de la U/Semestre 10/qa/untitled2/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{A62344EB-969A-1044-9EC4-07B9E48AF24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFEA7E19-BAB3-5D4F-9D4B-35FFEF4101AC}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{A62344EB-969A-1044-9EC4-07B9E48AF24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78DBE99C-8C4D-0A43-9873-F450AF8F57BA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{040C5902-4C25-1B49-BE38-6D6AB5496BB2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{040C5902-4C25-1B49-BE38-6D6AB5496BB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,15 +54,9 @@
     <t>iMac</t>
   </si>
   <si>
-    <t>Samsung galaxy tab 10.1</t>
-  </si>
-  <si>
     <t>Phones &amp; PDAs</t>
   </si>
   <si>
-    <t>HTC</t>
-  </si>
-  <si>
     <t>Desktops</t>
   </si>
   <si>
@@ -127,6 +121,12 @@
   </si>
   <si>
     <t>sistemas &gt;&gt; telecos</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Tab 10.1</t>
+  </si>
+  <si>
+    <t>HTC Touch HD</t>
   </si>
 </sst>
 </file>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DD0BE28-42CE-C143-88B0-940F9498A7DD}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScale="358" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="358" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,7 +538,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -549,18 +549,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C712E3-4710-8243-9AB4-09A54932DFB0}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="156" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -586,82 +586,82 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se añade el flujo completo de compra
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fa8db44bbb22994a/Escritorio/Cosas/Cosas de la U/Semestre 10/qa/untitled2/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{A62344EB-969A-1044-9EC4-07B9E48AF24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78DBE99C-8C4D-0A43-9873-F450AF8F57BA}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="8_{A62344EB-969A-1044-9EC4-07B9E48AF24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E5E1ED0-FB57-EA42-AB88-9B4CCD449EC4}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{040C5902-4C25-1B49-BE38-6D6AB5496BB2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{040C5902-4C25-1B49-BE38-6D6AB5496BB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>categoria</t>
   </si>
@@ -127,6 +128,18 @@
   </si>
   <si>
     <t>HTC Touch HD</t>
+  </si>
+  <si>
+    <t>Nikon D300</t>
+  </si>
+  <si>
+    <t>Cameras</t>
+  </si>
+  <si>
+    <t>iPhone</t>
+  </si>
+  <si>
+    <t>fail</t>
   </si>
 </sst>
 </file>
@@ -513,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DD0BE28-42CE-C143-88B0-940F9498A7DD}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="358" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="358" workbookViewId="0">
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,6 +574,22 @@
       </c>
       <c r="C4" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -674,4 +703,77 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE06D5E7-5A78-9648-A75D-D702BA6B1763}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="266" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
minor change to excel file data
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fa8db44bbb22994a/Escritorio/Cosas/Cosas de la U/Semestre 10/qa/untitled2/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="8_{A62344EB-969A-1044-9EC4-07B9E48AF24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E5E1ED0-FB57-EA42-AB88-9B4CCD449EC4}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{A62344EB-969A-1044-9EC4-07B9E48AF24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CD23C6A-23FF-2940-BE50-8402763C057B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{040C5902-4C25-1B49-BE38-6D6AB5496BB2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{040C5902-4C25-1B49-BE38-6D6AB5496BB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>categoria</t>
   </si>
@@ -140,6 +140,24 @@
   </si>
   <si>
     <t>fail</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>telefone</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>confirm password</t>
   </si>
 </sst>
 </file>
@@ -529,7 +547,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="358" workbookViewId="0">
-      <selection sqref="A1:C6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -599,10 +617,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C712E3-4710-8243-9AB4-09A54932DFB0}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScale="156" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,95 +629,116 @@
     <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>27</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" xr:uid="{09D72275-184F-224D-B54E-1F4B4EA3545D}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{06751F77-A1F5-574D-8355-680E420DD6A2}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{44807B0A-72EB-9546-A33B-D40C1F6DF325}"/>
-    <hyperlink ref="D3" r:id="rId4" display="https://youtu.be/SBs455jwb8w?si=EOOIHk3wa9iFf3z5" xr:uid="{866112D8-7B8F-944D-8D28-4663271A653B}"/>
-    <hyperlink ref="C4" r:id="rId5" xr:uid="{21888DB7-2585-EA48-9967-EFB3A82B2BD7}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{09D72275-184F-224D-B54E-1F4B4EA3545D}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{06751F77-A1F5-574D-8355-680E420DD6A2}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{44807B0A-72EB-9546-A33B-D40C1F6DF325}"/>
+    <hyperlink ref="D4" r:id="rId4" display="https://youtu.be/SBs455jwb8w?si=EOOIHk3wa9iFf3z5" xr:uid="{866112D8-7B8F-944D-8D28-4663271A653B}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{21888DB7-2585-EA48-9967-EFB3A82B2BD7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -709,7 +748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE06D5E7-5A78-9648-A75D-D702BA6B1763}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="266" workbookViewId="0">
+    <sheetView zoomScale="266" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>